<commit_message>
Adding view files button
</commit_message>
<xml_diff>
--- a/pricepopulate/data/data.xlsx
+++ b/pricepopulate/data/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="426">
   <si>
     <t>2902 N Caroline</t>
   </si>
@@ -820,202 +820,301 @@
     <t>31-13-03</t>
   </si>
   <si>
-    <t>$28077</t>
-  </si>
-  <si>
-    <t>$31120</t>
-  </si>
-  <si>
-    <t>$32588</t>
-  </si>
-  <si>
-    <t>$53332</t>
-  </si>
-  <si>
-    <t>$44056</t>
-  </si>
-  <si>
-    <t>$68887</t>
-  </si>
-  <si>
-    <t>$82680</t>
-  </si>
-  <si>
-    <t>$85285</t>
-  </si>
-  <si>
-    <t>$68967</t>
-  </si>
-  <si>
-    <t>$73864</t>
-  </si>
-  <si>
-    <t>$57747</t>
-  </si>
-  <si>
-    <t>$92825</t>
-  </si>
-  <si>
-    <t>$62794</t>
+    <t>$28309</t>
+  </si>
+  <si>
+    <t>$42,000</t>
+  </si>
+  <si>
+    <t>$30893</t>
+  </si>
+  <si>
+    <t>$30,000</t>
+  </si>
+  <si>
+    <t>$32475</t>
+  </si>
+  <si>
+    <t>Not Found</t>
+  </si>
+  <si>
+    <t>$53722</t>
+  </si>
+  <si>
+    <t>$44625</t>
+  </si>
+  <si>
+    <t>$68831</t>
+  </si>
+  <si>
+    <t>$66,000</t>
+  </si>
+  <si>
+    <t>$83866</t>
+  </si>
+  <si>
+    <t>$81,000</t>
+  </si>
+  <si>
+    <t>$86526</t>
+  </si>
+  <si>
+    <t>$69472</t>
+  </si>
+  <si>
+    <t>$73695</t>
+  </si>
+  <si>
+    <t>$78,000</t>
+  </si>
+  <si>
+    <t>$57690</t>
+  </si>
+  <si>
+    <t>$69,000</t>
+  </si>
+  <si>
+    <t>$92352</t>
+  </si>
+  <si>
+    <t>$89,000</t>
+  </si>
+  <si>
+    <t>$63507</t>
+  </si>
+  <si>
+    <t>$135,000</t>
   </si>
   <si>
     <t>Not found</t>
   </si>
   <si>
-    <t>$92600</t>
-  </si>
-  <si>
-    <t>$79822</t>
-  </si>
-  <si>
-    <t>$74570</t>
-  </si>
-  <si>
-    <t>$66883</t>
-  </si>
-  <si>
-    <t>$40014</t>
-  </si>
-  <si>
-    <t>$67433</t>
-  </si>
-  <si>
-    <t>$65539</t>
-  </si>
-  <si>
-    <t>$61227</t>
-  </si>
-  <si>
-    <t>$55236</t>
-  </si>
-  <si>
-    <t>$45799</t>
-  </si>
-  <si>
-    <t>$87677</t>
-  </si>
-  <si>
-    <t>$55799</t>
-  </si>
-  <si>
-    <t>$71498</t>
-  </si>
-  <si>
-    <t>$47786</t>
-  </si>
-  <si>
-    <t>$96622</t>
-  </si>
-  <si>
-    <t>$50897</t>
-  </si>
-  <si>
-    <t>$48909</t>
-  </si>
-  <si>
-    <t>$109127</t>
-  </si>
-  <si>
-    <t>$62032</t>
-  </si>
-  <si>
-    <t>$78448</t>
-  </si>
-  <si>
-    <t>$48508</t>
-  </si>
-  <si>
-    <t>$75853</t>
-  </si>
-  <si>
-    <t>$61356</t>
-  </si>
-  <si>
-    <t>$38795</t>
-  </si>
-  <si>
-    <t>$54160</t>
-  </si>
-  <si>
-    <t>$72576</t>
-  </si>
-  <si>
-    <t>$55449</t>
-  </si>
-  <si>
-    <t>$32978</t>
-  </si>
-  <si>
-    <t>$94814</t>
-  </si>
-  <si>
-    <t>$72866</t>
-  </si>
-  <si>
-    <t>$81249</t>
-  </si>
-  <si>
-    <t>$72767</t>
-  </si>
-  <si>
-    <t>$55574</t>
-  </si>
-  <si>
-    <t>$63934</t>
-  </si>
-  <si>
-    <t>$48824</t>
-  </si>
-  <si>
-    <t>$58163</t>
-  </si>
-  <si>
-    <t>$59839</t>
-  </si>
-  <si>
-    <t>$81907</t>
-  </si>
-  <si>
-    <t>$73219</t>
-  </si>
-  <si>
-    <t>$62016</t>
-  </si>
-  <si>
-    <t>$62960</t>
-  </si>
-  <si>
-    <t>$48984</t>
-  </si>
-  <si>
-    <t>$50107</t>
-  </si>
-  <si>
-    <t>$103264</t>
-  </si>
-  <si>
-    <t>$66477</t>
-  </si>
-  <si>
-    <t>$67187</t>
-  </si>
-  <si>
-    <t>$44967</t>
-  </si>
-  <si>
-    <t>$61803</t>
-  </si>
-  <si>
-    <t>$35765</t>
-  </si>
-  <si>
-    <t>$169107</t>
-  </si>
-  <si>
-    <t>$60426</t>
-  </si>
-  <si>
-    <t>$101753</t>
+    <t>$89166</t>
+  </si>
+  <si>
+    <t>$78882</t>
+  </si>
+  <si>
+    <t>$74837</t>
+  </si>
+  <si>
+    <t>$57,000</t>
+  </si>
+  <si>
+    <t>$67747</t>
+  </si>
+  <si>
+    <t>$39835</t>
+  </si>
+  <si>
+    <t>$67557</t>
+  </si>
+  <si>
+    <t>$58,000</t>
+  </si>
+  <si>
+    <t>$66176</t>
+  </si>
+  <si>
+    <t>$61425</t>
+  </si>
+  <si>
+    <t>$56454</t>
+  </si>
+  <si>
+    <t>$45801</t>
+  </si>
+  <si>
+    <t>$85294</t>
+  </si>
+  <si>
+    <t>$111,000</t>
+  </si>
+  <si>
+    <t>$54053</t>
+  </si>
+  <si>
+    <t>$61,000</t>
+  </si>
+  <si>
+    <t>$70683</t>
+  </si>
+  <si>
+    <t>$65,000</t>
+  </si>
+  <si>
+    <t>$48389</t>
+  </si>
+  <si>
+    <t>$47,000</t>
+  </si>
+  <si>
+    <t>$97182</t>
+  </si>
+  <si>
+    <t>$51721</t>
+  </si>
+  <si>
+    <t>$62,000</t>
+  </si>
+  <si>
+    <t>$48803</t>
+  </si>
+  <si>
+    <t>$56,000</t>
+  </si>
+  <si>
+    <t>$108005</t>
+  </si>
+  <si>
+    <t>$62128</t>
+  </si>
+  <si>
+    <t>$38,000</t>
+  </si>
+  <si>
+    <t>$76657</t>
+  </si>
+  <si>
+    <t>$55,000</t>
+  </si>
+  <si>
+    <t>$50359</t>
+  </si>
+  <si>
+    <t>$75,000</t>
+  </si>
+  <si>
+    <t>$75485</t>
+  </si>
+  <si>
+    <t>$114,000</t>
+  </si>
+  <si>
+    <t>$60969</t>
+  </si>
+  <si>
+    <t>$38162</t>
+  </si>
+  <si>
+    <t>$55815</t>
+  </si>
+  <si>
+    <t>$71549</t>
+  </si>
+  <si>
+    <t>$102,000</t>
+  </si>
+  <si>
+    <t>$55880</t>
+  </si>
+  <si>
+    <t>$49,000</t>
+  </si>
+  <si>
+    <t>$32880</t>
+  </si>
+  <si>
+    <t>$95502</t>
+  </si>
+  <si>
+    <t>$87,000</t>
+  </si>
+  <si>
+    <t>$70119</t>
+  </si>
+  <si>
+    <t>$82782</t>
+  </si>
+  <si>
+    <t>$73155</t>
+  </si>
+  <si>
+    <t>$56869</t>
+  </si>
+  <si>
+    <t>$64391</t>
+  </si>
+  <si>
+    <t>$52,000</t>
+  </si>
+  <si>
+    <t>$49109</t>
+  </si>
+  <si>
+    <t>$59184</t>
+  </si>
+  <si>
+    <t>$77,000</t>
+  </si>
+  <si>
+    <t>$59300</t>
+  </si>
+  <si>
+    <t>$53,000</t>
+  </si>
+  <si>
+    <t>$82346</t>
+  </si>
+  <si>
+    <t>$70,000</t>
+  </si>
+  <si>
+    <t>$72107</t>
+  </si>
+  <si>
+    <t>$62182</t>
+  </si>
+  <si>
+    <t>$60879</t>
+  </si>
+  <si>
+    <t>$48646</t>
+  </si>
+  <si>
+    <t>$50220</t>
+  </si>
+  <si>
+    <t>$39,000</t>
+  </si>
+  <si>
+    <t>$103394</t>
+  </si>
+  <si>
+    <t>$64634</t>
+  </si>
+  <si>
+    <t>$66828</t>
+  </si>
+  <si>
+    <t>$80,000</t>
+  </si>
+  <si>
+    <t>$43869</t>
+  </si>
+  <si>
+    <t>$35,000</t>
+  </si>
+  <si>
+    <t>$63144</t>
+  </si>
+  <si>
+    <t>$115,000</t>
+  </si>
+  <si>
+    <t>$36249</t>
+  </si>
+  <si>
+    <t>$36,000</t>
+  </si>
+  <si>
+    <t>$167234</t>
+  </si>
+  <si>
+    <t>$60642</t>
+  </si>
+  <si>
+    <t>$104151</t>
   </si>
   <si>
     <t>Yield</t>
@@ -9834,8 +9933,8 @@
       <c r="T4" s="306" t="s">
         <v>261</v>
       </c>
-      <c r="U4" s="306" t="n">
-        <v>34000</v>
+      <c r="U4" s="306" t="s">
+        <v>262</v>
       </c>
       <c r="V4" s="306" t="n">
         <v>43000</v>
@@ -9917,10 +10016,10 @@
         <v/>
       </c>
       <c r="T5" s="306" t="s">
-        <v>262</v>
-      </c>
-      <c r="U5" s="306" t="n">
-        <v>31000</v>
+        <v>263</v>
+      </c>
+      <c r="U5" s="306" t="s">
+        <v>264</v>
       </c>
       <c r="V5" s="306" t="n">
         <v>58000</v>
@@ -10002,9 +10101,11 @@
         <v/>
       </c>
       <c r="T6" s="306" t="s">
-        <v>263</v>
-      </c>
-      <c r="U6" s="306" t="n"/>
+        <v>265</v>
+      </c>
+      <c r="U6" s="306" t="s">
+        <v>266</v>
+      </c>
       <c r="V6" s="306" t="n">
         <v>51150</v>
       </c>
@@ -10085,9 +10186,11 @@
         <v/>
       </c>
       <c r="T7" s="189" t="s">
-        <v>264</v>
-      </c>
-      <c r="U7" s="189" t="n"/>
+        <v>267</v>
+      </c>
+      <c r="U7" s="189" t="s">
+        <v>266</v>
+      </c>
       <c r="V7" s="189" t="n">
         <v>56000</v>
       </c>
@@ -10168,9 +10271,11 @@
         <v/>
       </c>
       <c r="T8" s="189" t="s">
-        <v>265</v>
-      </c>
-      <c r="U8" s="189" t="n"/>
+        <v>268</v>
+      </c>
+      <c r="U8" s="189" t="s">
+        <v>266</v>
+      </c>
       <c r="V8" s="189" t="n">
         <v>49000</v>
       </c>
@@ -10251,10 +10356,10 @@
         <v/>
       </c>
       <c r="T9" s="189" t="s">
-        <v>266</v>
-      </c>
-      <c r="U9" s="189" t="n">
-        <v>67000</v>
+        <v>269</v>
+      </c>
+      <c r="U9" s="189" t="s">
+        <v>270</v>
       </c>
       <c r="V9" s="189" t="n">
         <v>48000</v>
@@ -10336,10 +10441,10 @@
         <v/>
       </c>
       <c r="T10" s="306" t="s">
-        <v>267</v>
-      </c>
-      <c r="U10" s="306" t="n">
-        <v>62000</v>
+        <v>271</v>
+      </c>
+      <c r="U10" s="306" t="s">
+        <v>272</v>
       </c>
       <c r="V10" s="306" t="n">
         <v>78000</v>
@@ -10421,10 +10526,10 @@
         <v/>
       </c>
       <c r="T11" s="306" t="s">
-        <v>268</v>
-      </c>
-      <c r="U11" s="306" t="n">
-        <v>78000</v>
+        <v>273</v>
+      </c>
+      <c r="U11" s="306" t="s">
+        <v>266</v>
       </c>
       <c r="V11" s="306" t="n">
         <v>84000</v>
@@ -10506,10 +10611,10 @@
         <v/>
       </c>
       <c r="T12" s="189" t="s">
-        <v>269</v>
-      </c>
-      <c r="U12" s="189" t="n">
-        <v>60000</v>
+        <v>274</v>
+      </c>
+      <c r="U12" s="189" t="s">
+        <v>266</v>
       </c>
       <c r="V12" s="189" t="n">
         <v>77670</v>
@@ -10591,10 +10696,10 @@
         <v/>
       </c>
       <c r="T13" s="189" t="s">
-        <v>270</v>
-      </c>
-      <c r="U13" s="189" t="n">
-        <v>66000</v>
+        <v>275</v>
+      </c>
+      <c r="U13" s="189" t="s">
+        <v>276</v>
       </c>
       <c r="V13" s="189" t="n">
         <v>49000</v>
@@ -10674,10 +10779,10 @@
         <v/>
       </c>
       <c r="T14" s="189" t="s">
-        <v>271</v>
-      </c>
-      <c r="U14" s="189" t="n">
-        <v>59000</v>
+        <v>277</v>
+      </c>
+      <c r="U14" s="189" t="s">
+        <v>278</v>
       </c>
       <c r="V14" s="189" t="n">
         <v>65680</v>
@@ -10759,10 +10864,10 @@
         <v/>
       </c>
       <c r="T15" s="189" t="s">
-        <v>272</v>
-      </c>
-      <c r="U15" s="189" t="n">
-        <v>99000</v>
+        <v>279</v>
+      </c>
+      <c r="U15" s="189" t="s">
+        <v>280</v>
       </c>
       <c r="V15" s="189" t="n">
         <v>115370</v>
@@ -10844,10 +10949,10 @@
         <v/>
       </c>
       <c r="T16" s="306" t="s">
-        <v>273</v>
-      </c>
-      <c r="U16" s="306" t="n">
-        <v>98000</v>
+        <v>281</v>
+      </c>
+      <c r="U16" s="306" t="s">
+        <v>282</v>
       </c>
       <c r="V16" s="306" t="n">
         <v>91000</v>
@@ -10929,9 +11034,11 @@
         <v/>
       </c>
       <c r="T17" s="189" t="s">
-        <v>274</v>
-      </c>
-      <c r="U17" s="189" t="n"/>
+        <v>283</v>
+      </c>
+      <c r="U17" s="189" t="s">
+        <v>266</v>
+      </c>
       <c r="V17" s="189" t="n">
         <v>14640</v>
       </c>
@@ -11012,9 +11119,11 @@
         <v/>
       </c>
       <c r="T18" s="306" t="s">
-        <v>274</v>
-      </c>
-      <c r="U18" s="306" t="n"/>
+        <v>283</v>
+      </c>
+      <c r="U18" s="306" t="s">
+        <v>266</v>
+      </c>
       <c r="V18" s="306" t="n"/>
       <c r="W18" s="306">
         <f>AVERAGE(T18:V18)</f>
@@ -11089,9 +11198,11 @@
         <v/>
       </c>
       <c r="T19" s="189" t="s">
-        <v>275</v>
-      </c>
-      <c r="U19" s="189" t="n"/>
+        <v>284</v>
+      </c>
+      <c r="U19" s="189" t="s">
+        <v>266</v>
+      </c>
       <c r="V19" s="189" t="n">
         <v>68000</v>
       </c>
@@ -11172,9 +11283,11 @@
         <v/>
       </c>
       <c r="T20" s="189" t="s">
-        <v>276</v>
-      </c>
-      <c r="U20" s="189" t="n"/>
+        <v>285</v>
+      </c>
+      <c r="U20" s="189" t="s">
+        <v>266</v>
+      </c>
       <c r="V20" s="189" t="n">
         <v>44000</v>
       </c>
@@ -11255,10 +11368,10 @@
         <v/>
       </c>
       <c r="T21" s="306" t="s">
-        <v>277</v>
-      </c>
-      <c r="U21" s="306" t="n">
-        <v>91000</v>
+        <v>286</v>
+      </c>
+      <c r="U21" s="306" t="s">
+        <v>287</v>
       </c>
       <c r="V21" s="306" t="n">
         <v>80900</v>
@@ -11340,9 +11453,11 @@
         <v/>
       </c>
       <c r="T22" s="306" t="s">
-        <v>278</v>
-      </c>
-      <c r="U22" s="306" t="n"/>
+        <v>288</v>
+      </c>
+      <c r="U22" s="306" t="s">
+        <v>266</v>
+      </c>
       <c r="V22" s="306" t="n"/>
       <c r="W22" s="306">
         <f>AVERAGE(T22:V22)</f>
@@ -11421,10 +11536,10 @@
         <v/>
       </c>
       <c r="T23" s="306" t="s">
-        <v>279</v>
-      </c>
-      <c r="U23" s="306" t="n">
-        <v>34000</v>
+        <v>289</v>
+      </c>
+      <c r="U23" s="306" t="s">
+        <v>262</v>
       </c>
       <c r="V23" s="306" t="n">
         <v>45000</v>
@@ -11506,10 +11621,10 @@
         <v/>
       </c>
       <c r="T24" s="306" t="s">
-        <v>280</v>
-      </c>
-      <c r="U24" s="306" t="n">
-        <v>39000</v>
+        <v>290</v>
+      </c>
+      <c r="U24" s="306" t="s">
+        <v>291</v>
       </c>
       <c r="V24" s="306" t="n">
         <v>58000</v>
@@ -11591,9 +11706,11 @@
         <v/>
       </c>
       <c r="T25" s="189" t="s">
-        <v>281</v>
-      </c>
-      <c r="U25" s="189" t="n"/>
+        <v>292</v>
+      </c>
+      <c r="U25" s="189" t="s">
+        <v>266</v>
+      </c>
       <c r="V25" s="189" t="n"/>
       <c r="W25" s="189">
         <f>AVERAGE(T25:V25)</f>
@@ -11672,9 +11789,11 @@
         <v/>
       </c>
       <c r="T26" s="306" t="s">
-        <v>274</v>
-      </c>
-      <c r="U26" s="306" t="n"/>
+        <v>283</v>
+      </c>
+      <c r="U26" s="306" t="s">
+        <v>266</v>
+      </c>
       <c r="V26" s="306" t="n"/>
       <c r="W26" s="306">
         <f>AVERAGE(T26:V26)</f>
@@ -11749,9 +11868,11 @@
         <v/>
       </c>
       <c r="T27" s="306" t="s">
-        <v>282</v>
-      </c>
-      <c r="U27" s="306" t="n"/>
+        <v>293</v>
+      </c>
+      <c r="U27" s="306" t="s">
+        <v>266</v>
+      </c>
       <c r="V27" s="306" t="n"/>
       <c r="W27" s="306">
         <f>AVERAGE(T27:V27)</f>
@@ -11832,9 +11953,11 @@
         <v/>
       </c>
       <c r="T28" s="306" t="s">
-        <v>274</v>
-      </c>
-      <c r="U28" s="306" t="n"/>
+        <v>283</v>
+      </c>
+      <c r="U28" s="306" t="s">
+        <v>266</v>
+      </c>
       <c r="V28" s="306" t="n">
         <v>39000</v>
       </c>
@@ -11913,9 +12036,11 @@
         <v/>
       </c>
       <c r="T29" s="189" t="s">
-        <v>283</v>
-      </c>
-      <c r="U29" s="189" t="n"/>
+        <v>294</v>
+      </c>
+      <c r="U29" s="189" t="s">
+        <v>266</v>
+      </c>
       <c r="V29" s="189" t="n">
         <v>61000</v>
       </c>
@@ -11994,9 +12119,11 @@
         <v/>
       </c>
       <c r="T30" s="306" t="s">
-        <v>274</v>
-      </c>
-      <c r="U30" s="306" t="n"/>
+        <v>283</v>
+      </c>
+      <c r="U30" s="306" t="s">
+        <v>266</v>
+      </c>
       <c r="V30" s="306" t="n"/>
       <c r="W30" s="306">
         <f>AVERAGE(T30:V30)</f>
@@ -12071,10 +12198,10 @@
         <v/>
       </c>
       <c r="T31" s="306" t="s">
-        <v>284</v>
-      </c>
-      <c r="U31" s="306" t="n">
-        <v>49000</v>
+        <v>295</v>
+      </c>
+      <c r="U31" s="306" t="s">
+        <v>291</v>
       </c>
       <c r="V31" s="306" t="n">
         <v>40000</v>
@@ -12156,9 +12283,11 @@
         <v/>
       </c>
       <c r="T32" s="189" t="s">
-        <v>285</v>
-      </c>
-      <c r="U32" s="189" t="n"/>
+        <v>296</v>
+      </c>
+      <c r="U32" s="189" t="s">
+        <v>297</v>
+      </c>
       <c r="V32" s="189" t="n">
         <v>48000</v>
       </c>
@@ -12241,10 +12370,10 @@
         <v/>
       </c>
       <c r="T33" s="189" t="s">
-        <v>286</v>
-      </c>
-      <c r="U33" s="189" t="n">
-        <v>45000</v>
+        <v>298</v>
+      </c>
+      <c r="U33" s="189" t="s">
+        <v>299</v>
       </c>
       <c r="V33" s="189" t="n">
         <v>63390</v>
@@ -12328,9 +12457,11 @@
         <v/>
       </c>
       <c r="T34" s="306" t="s">
-        <v>287</v>
-      </c>
-      <c r="U34" s="306" t="n"/>
+        <v>300</v>
+      </c>
+      <c r="U34" s="306" t="s">
+        <v>301</v>
+      </c>
       <c r="V34" s="306" t="n"/>
       <c r="W34" s="306">
         <f>AVERAGE(T34:V34)</f>
@@ -12409,9 +12540,11 @@
         <v/>
       </c>
       <c r="T35" s="306" t="s">
-        <v>274</v>
-      </c>
-      <c r="U35" s="306" t="n"/>
+        <v>283</v>
+      </c>
+      <c r="U35" s="306" t="s">
+        <v>266</v>
+      </c>
       <c r="V35" s="306" t="n"/>
       <c r="W35" s="306">
         <f>AVERAGE(T35:V35)</f>
@@ -12486,9 +12619,11 @@
         <v/>
       </c>
       <c r="T36" s="306" t="s">
-        <v>288</v>
-      </c>
-      <c r="U36" s="306" t="n"/>
+        <v>302</v>
+      </c>
+      <c r="U36" s="306" t="s">
+        <v>303</v>
+      </c>
       <c r="V36" s="306" t="n"/>
       <c r="W36" s="306">
         <f>AVERAGE(T36:V36)</f>
@@ -12563,9 +12698,11 @@
         <v/>
       </c>
       <c r="T37" s="306" t="s">
-        <v>289</v>
-      </c>
-      <c r="U37" s="306" t="n"/>
+        <v>304</v>
+      </c>
+      <c r="U37" s="306" t="s">
+        <v>299</v>
+      </c>
       <c r="V37" s="306" t="n"/>
       <c r="W37" s="306">
         <f>AVERAGE(T37:V37)</f>
@@ -12642,9 +12779,11 @@
         <v/>
       </c>
       <c r="T38" s="306" t="s">
-        <v>290</v>
-      </c>
-      <c r="U38" s="306" t="n"/>
+        <v>305</v>
+      </c>
+      <c r="U38" s="306" t="s">
+        <v>306</v>
+      </c>
       <c r="V38" s="306" t="n"/>
       <c r="W38" s="306">
         <f>AVERAGE(T38:V38)</f>
@@ -12721,9 +12860,11 @@
         <v/>
       </c>
       <c r="T39" s="306" t="s">
-        <v>291</v>
-      </c>
-      <c r="U39" s="306" t="n"/>
+        <v>307</v>
+      </c>
+      <c r="U39" s="306" t="s">
+        <v>308</v>
+      </c>
       <c r="V39" s="306" t="n"/>
       <c r="W39" s="306">
         <f>AVERAGE(T39:V39)</f>
@@ -12798,9 +12939,11 @@
         <v/>
       </c>
       <c r="T40" s="306" t="s">
-        <v>292</v>
-      </c>
-      <c r="U40" s="306" t="n"/>
+        <v>309</v>
+      </c>
+      <c r="U40" s="306" t="s">
+        <v>270</v>
+      </c>
       <c r="V40" s="306" t="n"/>
       <c r="W40" s="306">
         <f>AVERAGE(T40:V40)</f>
@@ -12877,10 +13020,10 @@
         <v/>
       </c>
       <c r="T41" s="189" t="s">
-        <v>293</v>
-      </c>
-      <c r="U41" s="189" t="n">
-        <v>37000</v>
+        <v>310</v>
+      </c>
+      <c r="U41" s="189" t="s">
+        <v>311</v>
       </c>
       <c r="V41" s="189" t="n">
         <v>41000</v>
@@ -12964,10 +13107,10 @@
         <v/>
       </c>
       <c r="T42" s="306" t="s">
-        <v>294</v>
-      </c>
-      <c r="U42" s="306" t="n">
-        <v>65000</v>
+        <v>312</v>
+      </c>
+      <c r="U42" s="306" t="s">
+        <v>313</v>
       </c>
       <c r="V42" s="306" t="n">
         <v>60000</v>
@@ -13046,9 +13189,11 @@
         <v/>
       </c>
       <c r="T43" s="306" t="s">
-        <v>295</v>
-      </c>
-      <c r="U43" s="306" t="n"/>
+        <v>314</v>
+      </c>
+      <c r="U43" s="306" t="s">
+        <v>315</v>
+      </c>
       <c r="V43" s="306" t="n"/>
       <c r="W43" s="306">
         <f>AVERAGE(T43:V43)</f>
@@ -13125,9 +13270,11 @@
         <v/>
       </c>
       <c r="T44" s="306" t="s">
-        <v>296</v>
-      </c>
-      <c r="U44" s="306" t="n"/>
+        <v>316</v>
+      </c>
+      <c r="U44" s="306" t="s">
+        <v>317</v>
+      </c>
       <c r="V44" s="306" t="n"/>
       <c r="W44" s="306">
         <f>AVERAGE(T44:V44)</f>
@@ -13202,9 +13349,11 @@
         <v/>
       </c>
       <c r="T45" s="306" t="s">
-        <v>297</v>
-      </c>
-      <c r="U45" s="306" t="n"/>
+        <v>318</v>
+      </c>
+      <c r="U45" s="306" t="s">
+        <v>308</v>
+      </c>
       <c r="V45" s="306" t="n"/>
       <c r="W45" s="306">
         <f>AVERAGE(T45:V45)</f>
@@ -13279,9 +13428,11 @@
         <v/>
       </c>
       <c r="T46" s="189" t="s">
-        <v>298</v>
-      </c>
-      <c r="U46" s="189" t="n"/>
+        <v>319</v>
+      </c>
+      <c r="U46" s="189" t="s">
+        <v>266</v>
+      </c>
       <c r="V46" s="189" t="n">
         <v>57000</v>
       </c>
@@ -13362,10 +13513,10 @@
         <v/>
       </c>
       <c r="T47" s="306" t="s">
-        <v>299</v>
-      </c>
-      <c r="U47" s="306" t="n">
-        <v>64000</v>
+        <v>320</v>
+      </c>
+      <c r="U47" s="306" t="s">
+        <v>315</v>
       </c>
       <c r="V47" s="306" t="n">
         <v>67000</v>
@@ -13447,9 +13598,11 @@
         <v/>
       </c>
       <c r="T48" s="306" t="s">
-        <v>300</v>
-      </c>
-      <c r="U48" s="306" t="n"/>
+        <v>321</v>
+      </c>
+      <c r="U48" s="306" t="s">
+        <v>322</v>
+      </c>
       <c r="V48" s="306" t="n"/>
       <c r="W48" s="306">
         <f>AVERAGE(T48:V48)</f>
@@ -13524,9 +13677,11 @@
         <v/>
       </c>
       <c r="T49" s="306" t="s">
-        <v>301</v>
-      </c>
-      <c r="U49" s="306" t="n"/>
+        <v>323</v>
+      </c>
+      <c r="U49" s="306" t="s">
+        <v>324</v>
+      </c>
       <c r="V49" s="306" t="n"/>
       <c r="W49" s="306">
         <f>AVERAGE(T49:V49)</f>
@@ -13601,9 +13756,11 @@
         <v/>
       </c>
       <c r="T50" s="306" t="s">
-        <v>302</v>
-      </c>
-      <c r="U50" s="306" t="n"/>
+        <v>325</v>
+      </c>
+      <c r="U50" s="306" t="s">
+        <v>266</v>
+      </c>
       <c r="V50" s="306" t="n"/>
       <c r="W50" s="306">
         <f>AVERAGE(T50:V50)</f>
@@ -13678,9 +13835,11 @@
         <v/>
       </c>
       <c r="T51" s="306" t="s">
-        <v>303</v>
-      </c>
-      <c r="U51" s="306" t="n"/>
+        <v>326</v>
+      </c>
+      <c r="U51" s="306" t="s">
+        <v>327</v>
+      </c>
       <c r="V51" s="306" t="n"/>
       <c r="W51" s="306">
         <f>AVERAGE(T51:V51)</f>
@@ -13755,9 +13914,11 @@
         <v/>
       </c>
       <c r="T52" s="306" t="s">
-        <v>304</v>
-      </c>
-      <c r="U52" s="306" t="n"/>
+        <v>328</v>
+      </c>
+      <c r="U52" s="306" t="s">
+        <v>266</v>
+      </c>
       <c r="V52" s="306" t="n"/>
       <c r="W52" s="306">
         <f>AVERAGE(T52:V52)</f>
@@ -13832,9 +13993,11 @@
         <v/>
       </c>
       <c r="T53" s="306" t="s">
-        <v>305</v>
-      </c>
-      <c r="U53" s="306" t="n"/>
+        <v>329</v>
+      </c>
+      <c r="U53" s="306" t="s">
+        <v>266</v>
+      </c>
       <c r="V53" s="306" t="n">
         <v>61000</v>
       </c>
@@ -13915,9 +14078,11 @@
         <v/>
       </c>
       <c r="T54" s="306" t="s">
-        <v>306</v>
-      </c>
-      <c r="U54" s="306" t="n"/>
+        <v>330</v>
+      </c>
+      <c r="U54" s="306" t="s">
+        <v>266</v>
+      </c>
       <c r="V54" s="306" t="n"/>
       <c r="W54" s="306">
         <f>AVERAGE(T54:V54)</f>
@@ -13992,10 +14157,10 @@
         <v/>
       </c>
       <c r="T55" s="361" t="s">
-        <v>307</v>
-      </c>
-      <c r="U55" s="361" t="n">
-        <v>45000</v>
+        <v>331</v>
+      </c>
+      <c r="U55" s="361" t="s">
+        <v>266</v>
       </c>
       <c r="V55" s="361" t="n">
         <v>45000</v>
@@ -14077,7 +14242,10 @@
         <v/>
       </c>
       <c r="T56" t="s">
-        <v>308</v>
+        <v>332</v>
+      </c>
+      <c r="U56" t="s">
+        <v>333</v>
       </c>
       <c r="W56" s="306">
         <f>AVERAGE(T56:V56)</f>
@@ -14150,7 +14318,10 @@
         <v/>
       </c>
       <c r="T57" t="s">
-        <v>309</v>
+        <v>334</v>
+      </c>
+      <c r="U57" t="s">
+        <v>324</v>
       </c>
       <c r="W57" s="306">
         <f>AVERAGE(T57:V57)</f>
@@ -14223,7 +14394,10 @@
         <v/>
       </c>
       <c r="T58" t="s">
-        <v>310</v>
+        <v>335</v>
+      </c>
+      <c r="U58" t="s">
+        <v>336</v>
       </c>
       <c r="W58" s="306">
         <f>AVERAGE(T58:V58)</f>
@@ -14296,10 +14470,10 @@
         <v/>
       </c>
       <c r="T59" s="361" t="s">
-        <v>311</v>
-      </c>
-      <c r="U59" s="361" t="n">
-        <v>210000</v>
+        <v>337</v>
+      </c>
+      <c r="U59" s="361" t="s">
+        <v>338</v>
       </c>
       <c r="V59" s="361" t="n">
         <v>59000</v>
@@ -14381,7 +14555,10 @@
         <v/>
       </c>
       <c r="T60" t="s">
-        <v>312</v>
+        <v>339</v>
+      </c>
+      <c r="U60" t="s">
+        <v>340</v>
       </c>
       <c r="W60" s="306">
         <f>AVERAGE(T60:V60)</f>
@@ -14454,7 +14631,10 @@
         <v/>
       </c>
       <c r="T61" t="s">
-        <v>313</v>
+        <v>341</v>
+      </c>
+      <c r="U61" t="s">
+        <v>315</v>
       </c>
       <c r="W61" s="306">
         <f>AVERAGE(T61:V61)</f>
@@ -14527,7 +14707,10 @@
         <v/>
       </c>
       <c r="T62" t="s">
-        <v>314</v>
+        <v>342</v>
+      </c>
+      <c r="U62" t="s">
+        <v>324</v>
       </c>
       <c r="W62" s="308" t="n"/>
       <c r="X62" s="308" t="n"/>
@@ -14594,7 +14777,10 @@
         <v/>
       </c>
       <c r="T63" t="s">
-        <v>315</v>
+        <v>343</v>
+      </c>
+      <c r="U63" t="s">
+        <v>303</v>
       </c>
       <c r="W63" s="308" t="n"/>
       <c r="X63" s="308" t="n"/>
@@ -14661,7 +14847,10 @@
         <v/>
       </c>
       <c r="T64" t="s">
-        <v>316</v>
+        <v>344</v>
+      </c>
+      <c r="U64" t="s">
+        <v>266</v>
       </c>
       <c r="W64" s="308" t="n"/>
       <c r="X64" s="308" t="n"/>
@@ -14728,7 +14917,10 @@
         <v/>
       </c>
       <c r="T65" t="s">
-        <v>317</v>
+        <v>345</v>
+      </c>
+      <c r="U65" t="s">
+        <v>346</v>
       </c>
       <c r="W65" s="308" t="n"/>
       <c r="X65" s="308" t="n"/>
@@ -14795,7 +14987,10 @@
         <v/>
       </c>
       <c r="T66" t="s">
-        <v>318</v>
+        <v>347</v>
+      </c>
+      <c r="U66" t="s">
+        <v>266</v>
       </c>
       <c r="W66" s="308" t="n"/>
       <c r="X66" s="308" t="n"/>
@@ -14862,7 +15057,10 @@
         <v/>
       </c>
       <c r="T67" t="s">
-        <v>319</v>
+        <v>348</v>
+      </c>
+      <c r="U67" t="s">
+        <v>303</v>
       </c>
       <c r="W67" s="308" t="n"/>
       <c r="X67" s="308" t="n"/>
@@ -14929,7 +15127,10 @@
         <v/>
       </c>
       <c r="T68" t="s">
-        <v>320</v>
+        <v>349</v>
+      </c>
+      <c r="U68" t="s">
+        <v>350</v>
       </c>
       <c r="W68" s="308" t="n"/>
       <c r="X68" s="308" t="n"/>
@@ -14974,7 +15175,10 @@
       <c r="M69" s="308" t="n"/>
       <c r="N69" s="308" t="n"/>
       <c r="T69" t="s">
-        <v>274</v>
+        <v>283</v>
+      </c>
+      <c r="U69" t="s">
+        <v>266</v>
       </c>
       <c r="W69" s="308" t="n"/>
       <c r="X69" s="308" t="n"/>
@@ -15019,7 +15223,10 @@
       <c r="M70" s="308" t="n"/>
       <c r="N70" s="308" t="n"/>
       <c r="T70" t="s">
-        <v>321</v>
+        <v>351</v>
+      </c>
+      <c r="U70" t="s">
+        <v>352</v>
       </c>
       <c r="W70" s="308" t="n"/>
       <c r="X70" s="308" t="n"/>
@@ -15064,7 +15271,10 @@
       <c r="M71" s="308" t="n"/>
       <c r="N71" s="308" t="n"/>
       <c r="T71" t="s">
-        <v>322</v>
+        <v>353</v>
+      </c>
+      <c r="U71" t="s">
+        <v>354</v>
       </c>
       <c r="W71" s="308" t="n"/>
       <c r="X71" s="308" t="n"/>
@@ -15109,7 +15319,10 @@
       <c r="M72" s="308" t="n"/>
       <c r="N72" s="308" t="n"/>
       <c r="T72" t="s">
-        <v>274</v>
+        <v>283</v>
+      </c>
+      <c r="U72" t="s">
+        <v>266</v>
       </c>
       <c r="W72" s="308" t="n"/>
       <c r="X72" s="308" t="n"/>
@@ -15154,7 +15367,10 @@
       <c r="M73" s="308" t="n"/>
       <c r="N73" s="308" t="n"/>
       <c r="T73" t="s">
-        <v>323</v>
+        <v>355</v>
+      </c>
+      <c r="U73" t="s">
+        <v>356</v>
       </c>
       <c r="W73" s="308" t="n"/>
       <c r="X73" s="308" t="n"/>
@@ -15199,7 +15415,10 @@
       <c r="M74" s="308" t="n"/>
       <c r="N74" s="308" t="n"/>
       <c r="T74" t="s">
-        <v>324</v>
+        <v>357</v>
+      </c>
+      <c r="U74" t="s">
+        <v>287</v>
       </c>
       <c r="W74" s="308" t="n"/>
       <c r="X74" s="308" t="n"/>
@@ -15244,7 +15463,10 @@
       <c r="M75" s="308" t="n"/>
       <c r="N75" s="308" t="n"/>
       <c r="T75" t="s">
-        <v>325</v>
+        <v>358</v>
+      </c>
+      <c r="U75" t="s">
+        <v>266</v>
       </c>
       <c r="W75" s="308" t="n"/>
       <c r="X75" s="308" t="n"/>
@@ -15289,616 +15511,619 @@
       <c r="M76" s="308" t="n"/>
       <c r="N76" s="308" t="n"/>
       <c r="T76" t="s">
-        <v>326</v>
+        <v>359</v>
+      </c>
+      <c r="U76" t="s">
+        <v>266</v>
       </c>
       <c r="W76" s="308" t="n"/>
       <c r="X76" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="77" s="307" spans="1:28">
       <c r="T77" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W77" s="308" t="n"/>
       <c r="X77" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="78" s="307" spans="1:28">
       <c r="T78" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W78" s="308" t="n"/>
       <c r="X78" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="79" s="307" spans="1:28">
       <c r="T79" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W79" s="308" t="n"/>
       <c r="X79" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="80" s="307" spans="1:28">
       <c r="T80" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W80" s="308" t="n"/>
       <c r="X80" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="81" s="307" spans="1:28">
       <c r="T81" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W81" s="308" t="n"/>
       <c r="X81" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="82" s="307" spans="1:28">
       <c r="T82" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W82" s="308" t="n"/>
       <c r="X82" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="83" s="307" spans="1:28">
       <c r="T83" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W83" s="308" t="n"/>
       <c r="X83" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="84" s="307" spans="1:28">
       <c r="T84" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W84" s="308" t="n"/>
       <c r="X84" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="85" s="307" spans="1:28">
       <c r="T85" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W85" s="308" t="n"/>
       <c r="X85" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="86" s="307" spans="1:28">
       <c r="T86" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W86" s="308" t="n"/>
       <c r="X86" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="87" s="307" spans="1:28">
       <c r="T87" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W87" s="308" t="n"/>
       <c r="X87" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="88" s="307" spans="1:28">
       <c r="T88" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W88" s="308" t="n"/>
       <c r="X88" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="89" s="307" spans="1:28">
       <c r="T89" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W89" s="308" t="n"/>
       <c r="X89" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="90" s="307" spans="1:28">
       <c r="T90" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W90" s="308" t="n"/>
       <c r="X90" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="91" s="307" spans="1:28">
       <c r="T91" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W91" s="308" t="n"/>
       <c r="X91" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="92" s="307" spans="1:28">
       <c r="T92" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W92" s="308" t="n"/>
       <c r="X92" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="93" s="307" spans="1:28">
       <c r="T93" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W93" s="308" t="n"/>
       <c r="X93" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="94" s="307" spans="1:28">
       <c r="T94" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W94" s="308" t="n"/>
       <c r="X94" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="95" s="307" spans="1:28">
       <c r="T95" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W95" s="308" t="n"/>
       <c r="X95" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="96" s="307" spans="1:28">
       <c r="T96" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W96" s="308" t="n"/>
       <c r="X96" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="97" s="307" spans="1:28">
       <c r="T97" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W97" s="308" t="n"/>
       <c r="X97" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="98" s="307" spans="1:28">
       <c r="T98" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W98" s="308" t="n"/>
       <c r="X98" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="99" s="307" spans="1:28">
       <c r="T99" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W99" s="308" t="n"/>
       <c r="X99" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="100" s="307" spans="1:28">
       <c r="T100" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W100" s="308" t="n"/>
       <c r="X100" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="101" s="307" spans="1:28">
       <c r="T101" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W101" s="308" t="n"/>
       <c r="X101" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="102" s="307" spans="1:28">
       <c r="T102" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W102" s="308" t="n"/>
       <c r="X102" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="103" s="307" spans="1:28">
       <c r="T103" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W103" s="308" t="n"/>
       <c r="X103" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="104" s="307" spans="1:28">
       <c r="T104" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W104" s="308" t="n"/>
       <c r="X104" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="105" s="307" spans="1:28">
       <c r="T105" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W105" s="308" t="n"/>
       <c r="X105" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="106" s="307" spans="1:28">
       <c r="T106" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W106" s="308" t="n"/>
       <c r="X106" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="107" s="307" spans="1:28">
       <c r="T107" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W107" s="308" t="n"/>
       <c r="X107" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="108" s="307" spans="1:28">
       <c r="T108" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W108" s="308" t="n"/>
       <c r="X108" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="109" s="307" spans="1:28">
       <c r="T109" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W109" s="308" t="n"/>
       <c r="X109" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="110" s="307" spans="1:28">
       <c r="T110" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W110" s="308" t="n"/>
       <c r="X110" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="111" s="307" spans="1:28">
       <c r="T111" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W111" s="308" t="n"/>
       <c r="X111" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="112" s="307" spans="1:28">
       <c r="T112" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W112" s="308" t="n"/>
       <c r="X112" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="113" s="307" spans="1:28">
       <c r="T113" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W113" s="308" t="n"/>
       <c r="X113" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="114" s="307" spans="1:28">
       <c r="T114" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W114" s="308" t="n"/>
       <c r="X114" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="115" s="307" spans="1:28">
       <c r="T115" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W115" s="308" t="n"/>
       <c r="X115" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="116" s="307" spans="1:28">
       <c r="T116" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W116" s="308" t="n"/>
       <c r="X116" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="117" s="307" spans="1:28">
       <c r="T117" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W117" s="308" t="n"/>
       <c r="X117" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="118" s="307" spans="1:28">
       <c r="T118" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W118" s="308" t="n"/>
       <c r="X118" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="119" s="307" spans="1:28">
       <c r="T119" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W119" s="308" t="n"/>
       <c r="X119" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="120" s="307" spans="1:28">
       <c r="T120" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W120" s="308" t="n"/>
       <c r="X120" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="121" s="307" spans="1:28">
       <c r="T121" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W121" s="308" t="n"/>
       <c r="X121" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="122" s="307" spans="1:28">
       <c r="T122" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W122" s="308" t="n"/>
       <c r="X122" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="123" s="307" spans="1:28">
       <c r="T123" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W123" s="308" t="n"/>
       <c r="X123" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="124" s="307" spans="1:28">
       <c r="T124" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W124" s="308" t="n"/>
       <c r="X124" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="125" s="307" spans="1:28">
       <c r="T125" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W125" s="308" t="n"/>
       <c r="X125" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="126" s="307" spans="1:28">
       <c r="T126" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W126" s="308" t="n"/>
       <c r="X126" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="127" s="307" spans="1:28">
       <c r="T127" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W127" s="308" t="n"/>
       <c r="X127" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="128" s="307" spans="1:28">
       <c r="T128" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W128" s="308" t="n"/>
       <c r="X128" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="129" s="307" spans="1:28">
       <c r="T129" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W129" s="308" t="n"/>
       <c r="X129" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="130" s="307" spans="1:28">
       <c r="T130" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W130" s="308" t="n"/>
       <c r="X130" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="131" s="307" spans="1:28">
       <c r="T131" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W131" s="308" t="n"/>
       <c r="X131" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="132" s="307" spans="1:28">
       <c r="T132" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W132" s="308" t="n"/>
       <c r="X132" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="133" s="307" spans="1:28">
       <c r="T133" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W133" s="308" t="n"/>
       <c r="X133" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="134" s="307" spans="1:28">
       <c r="T134" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W134" s="308" t="n"/>
       <c r="X134" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="135" s="307" spans="1:28">
       <c r="T135" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W135" s="308" t="n"/>
       <c r="X135" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="136" s="307" spans="1:28">
       <c r="T136" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W136" s="308" t="n"/>
       <c r="X136" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="137" s="307" spans="1:28">
       <c r="T137" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W137" s="308" t="n"/>
       <c r="X137" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="138" s="307" spans="1:28">
       <c r="T138" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W138" s="308" t="n"/>
       <c r="X138" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="139" s="307" spans="1:28">
       <c r="T139" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W139" s="308" t="n"/>
       <c r="X139" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="140" s="307" spans="1:28">
       <c r="T140" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W140" s="308" t="n"/>
       <c r="X140" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="141" s="307" spans="1:28">
       <c r="T141" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W141" s="308" t="n"/>
       <c r="X141" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="142" s="307" spans="1:28">
       <c r="T142" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W142" s="308" t="n"/>
       <c r="X142" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="143" s="307" spans="1:28">
       <c r="T143" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W143" s="308" t="n"/>
       <c r="X143" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="144" s="307" spans="1:28">
       <c r="T144" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W144" s="308" t="n"/>
       <c r="X144" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="145" s="307" spans="1:28">
       <c r="T145" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W145" s="308" t="n"/>
       <c r="X145" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="146" s="307" spans="1:28">
       <c r="T146" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W146" s="308" t="n"/>
       <c r="X146" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="147" s="307" spans="1:28">
       <c r="T147" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W147" s="308" t="n"/>
       <c r="X147" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="148" s="307" spans="1:28">
       <c r="T148" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W148" s="308" t="n"/>
       <c r="X148" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="149" s="307" spans="1:28">
       <c r="T149" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W149" s="308" t="n"/>
       <c r="X149" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="150" s="307" spans="1:28">
       <c r="T150" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W150" s="308" t="n"/>
       <c r="X150" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="151" s="307" spans="1:28">
       <c r="T151" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W151" s="308" t="n"/>
       <c r="X151" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="152" s="307" spans="1:28">
       <c r="T152" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W152" s="308" t="n"/>
       <c r="X152" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="153" s="307" spans="1:28">
       <c r="T153" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W153" s="308" t="n"/>
       <c r="X153" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="154" s="307" spans="1:28">
       <c r="T154" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W154" s="308" t="n"/>
       <c r="X154" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="155" s="307" spans="1:28">
       <c r="T155" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W155" s="308" t="n"/>
       <c r="X155" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="156" s="307" spans="1:28">
       <c r="T156" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W156" s="308" t="n"/>
       <c r="X156" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="157" s="307" spans="1:28">
       <c r="T157" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W157" s="308" t="n"/>
       <c r="X157" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="158" s="307" spans="1:28">
       <c r="T158" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W158" s="308" t="n"/>
       <c r="X158" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="159" s="307" spans="1:28">
       <c r="T159" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W159" s="308" t="n"/>
       <c r="X159" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="160" s="307" spans="1:28">
       <c r="T160" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W160" s="308" t="n"/>
       <c r="X160" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="161" s="307" spans="1:28">
       <c r="T161" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W161" s="308" t="n"/>
       <c r="X161" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="162" s="307" spans="1:28">
       <c r="T162" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W162" s="308" t="n"/>
       <c r="X162" s="308" t="n"/>
     </row>
     <row customHeight="1" ht="20.25" r="163" s="307" spans="1:28">
       <c r="T163" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="W163" s="308" t="n"/>
       <c r="X163" s="308" t="n"/>
@@ -16161,7 +16386,7 @@
         <v>20</v>
       </c>
       <c r="Q3" s="64" t="s">
-        <v>327</v>
+        <v>360</v>
       </c>
       <c r="R3" s="64" t="s">
         <v>45</v>
@@ -16279,7 +16504,7 @@
         <v>950</v>
       </c>
       <c r="AA4" s="134" t="s">
-        <v>328</v>
+        <v>361</v>
       </c>
       <c r="AB4" s="21" t="s">
         <v>24</v>
@@ -16468,16 +16693,16 @@
         <v>2015090802</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>329</v>
+        <v>362</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>330</v>
+        <v>363</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>141</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>331</v>
+        <v>364</v>
       </c>
       <c r="F7" s="26" t="s">
         <v>4</v>
@@ -16554,16 +16779,16 @@
         <v>2015090843</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>332</v>
+        <v>365</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>333</v>
+        <v>366</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>334</v>
+        <v>367</v>
       </c>
       <c r="F8" s="26" t="s">
         <v>4</v>
@@ -16640,10 +16865,10 @@
         <v>2015062911</v>
       </c>
       <c r="B9" s="194" t="s">
-        <v>335</v>
+        <v>368</v>
       </c>
       <c r="C9" s="195" t="s">
-        <v>336</v>
+        <v>369</v>
       </c>
       <c r="D9" s="148" t="s">
         <v>2</v>
@@ -16715,7 +16940,7 @@
       </c>
       <c r="Z9" s="306" t="n"/>
       <c r="AA9" s="135" t="s">
-        <v>337</v>
+        <v>370</v>
       </c>
       <c r="AB9" s="21" t="s">
         <v>24</v>
@@ -16807,7 +17032,7 @@
         <v>1080</v>
       </c>
       <c r="AA10" s="200" t="s">
-        <v>338</v>
+        <v>371</v>
       </c>
       <c r="AB10" s="201" t="s">
         <v>24</v>
@@ -16977,7 +17202,7 @@
       </c>
       <c r="Z12" s="306" t="n"/>
       <c r="AA12" s="134" t="s">
-        <v>339</v>
+        <v>372</v>
       </c>
       <c r="AB12" s="21" t="s">
         <v>24</v>
@@ -16988,10 +17213,10 @@
         <v>2015062905</v>
       </c>
       <c r="B13" s="194" t="s">
-        <v>340</v>
+        <v>373</v>
       </c>
       <c r="C13" s="195" t="s">
-        <v>341</v>
+        <v>374</v>
       </c>
       <c r="D13" s="148" t="s">
         <v>228</v>
@@ -17077,13 +17302,13 @@
         <v>2015062913</v>
       </c>
       <c r="B14" s="203" t="s">
-        <v>342</v>
+        <v>375</v>
       </c>
       <c r="C14" s="204" t="s">
-        <v>343</v>
+        <v>376</v>
       </c>
       <c r="D14" s="205" t="s">
-        <v>344</v>
+        <v>377</v>
       </c>
       <c r="E14" s="205" t="n">
         <v>71282</v>
@@ -17238,7 +17463,7 @@
         <v>1150</v>
       </c>
       <c r="AA15" s="136" t="s">
-        <v>345</v>
+        <v>378</v>
       </c>
       <c r="AB15" s="43" t="s">
         <v>24</v>
@@ -17249,16 +17474,16 @@
         <v>2015090815</v>
       </c>
       <c r="B16" s="122" t="s">
-        <v>346</v>
+        <v>379</v>
       </c>
       <c r="C16" s="123" t="s">
-        <v>347</v>
+        <v>380</v>
       </c>
       <c r="D16" s="124" t="s">
-        <v>344</v>
+        <v>377</v>
       </c>
       <c r="E16" s="124" t="s">
-        <v>348</v>
+        <v>381</v>
       </c>
       <c r="F16" s="125" t="s">
         <v>4</v>
@@ -17486,10 +17711,10 @@
         <v>2015062912</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>349</v>
+        <v>382</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>350</v>
+        <v>383</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>28</v>
@@ -17565,10 +17790,10 @@
         <v>2015062907</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>351</v>
+        <v>384</v>
       </c>
       <c r="C20" s="80" t="s">
-        <v>352</v>
+        <v>385</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>2</v>
@@ -17644,16 +17869,16 @@
         <v>2015090819</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>353</v>
+        <v>386</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>354</v>
+        <v>387</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>228</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>355</v>
+        <v>388</v>
       </c>
       <c r="F21" s="26" t="s">
         <v>4</v>
@@ -17723,10 +17948,10 @@
         <v>2015062909</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>356</v>
+        <v>389</v>
       </c>
       <c r="C22" s="80" t="s">
-        <v>357</v>
+        <v>390</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>23</v>
@@ -17872,7 +18097,7 @@
       </c>
       <c r="Z23" s="306" t="n"/>
       <c r="AA23" s="134" t="s">
-        <v>358</v>
+        <v>391</v>
       </c>
       <c r="AB23" s="21" t="s">
         <v>24</v>
@@ -17883,10 +18108,10 @@
         <v>2015062903</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>359</v>
+        <v>392</v>
       </c>
       <c r="C24" s="80" t="s">
-        <v>360</v>
+        <v>393</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>2</v>
@@ -18032,7 +18257,7 @@
       </c>
       <c r="Z25" s="306" t="n"/>
       <c r="AA25" s="325" t="s">
-        <v>361</v>
+        <v>394</v>
       </c>
       <c r="AB25" s="43" t="s">
         <v>24</v>
@@ -18122,10 +18347,10 @@
         <v>2015062901</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>362</v>
+        <v>395</v>
       </c>
       <c r="C27" s="80" t="s">
-        <v>363</v>
+        <v>396</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>2</v>
@@ -18201,10 +18426,10 @@
         <v>36137</v>
       </c>
       <c r="B28" s="167" t="s">
-        <v>364</v>
+        <v>397</v>
       </c>
       <c r="C28" s="167" t="s">
-        <v>365</v>
+        <v>398</v>
       </c>
       <c r="D28" s="168" t="s">
         <v>106</v>
@@ -18361,7 +18586,7 @@
         <v>39921</v>
       </c>
       <c r="B30" s="77" t="s">
-        <v>366</v>
+        <v>399</v>
       </c>
       <c r="C30" s="77" t="s">
         <v>1</v>
@@ -18373,7 +18598,7 @@
         <v>46205</v>
       </c>
       <c r="F30" s="77" t="s">
-        <v>367</v>
+        <v>400</v>
       </c>
       <c r="G30" s="92" t="n">
         <v>41053</v>
@@ -18440,19 +18665,19 @@
         <v>55220</v>
       </c>
       <c r="B31" s="35" t="s">
-        <v>368</v>
+        <v>401</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>369</v>
+        <v>402</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>370</v>
+        <v>403</v>
       </c>
       <c r="E31" s="34" t="n">
         <v>23434</v>
       </c>
       <c r="F31" s="35" t="s">
-        <v>367</v>
+        <v>400</v>
       </c>
       <c r="G31" s="24" t="n">
         <v>41149</v>
@@ -18598,7 +18823,7 @@
         <v>55192</v>
       </c>
       <c r="B33" s="35" t="s">
-        <v>371</v>
+        <v>404</v>
       </c>
       <c r="C33" s="35" t="s">
         <v>208</v>
@@ -18679,10 +18904,10 @@
         <v>55167</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>372</v>
+        <v>405</v>
       </c>
       <c r="C34" s="35" t="s">
-        <v>373</v>
+        <v>406</v>
       </c>
       <c r="D34" s="34" t="s">
         <v>28</v>
@@ -18760,10 +18985,10 @@
         <v>39770</v>
       </c>
       <c r="B35" s="35" t="s">
-        <v>374</v>
+        <v>407</v>
       </c>
       <c r="C35" s="35" t="s">
-        <v>375</v>
+        <v>408</v>
       </c>
       <c r="D35" s="34" t="s">
         <v>124</v>
@@ -18841,10 +19066,10 @@
         <v>39833</v>
       </c>
       <c r="B36" s="35" t="s">
-        <v>376</v>
+        <v>409</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>377</v>
+        <v>410</v>
       </c>
       <c r="D36" s="34" t="s">
         <v>2</v>
@@ -18853,7 +19078,7 @@
         <v>47345</v>
       </c>
       <c r="F36" s="35" t="s">
-        <v>367</v>
+        <v>400</v>
       </c>
       <c r="G36" s="24" t="n">
         <v>41305</v>
@@ -18999,7 +19224,7 @@
         <v>50036</v>
       </c>
       <c r="B38" s="35" t="s">
-        <v>378</v>
+        <v>411</v>
       </c>
       <c r="C38" s="35" t="s">
         <v>254</v>
@@ -19161,10 +19386,10 @@
         <v>55175</v>
       </c>
       <c r="B40" s="35" t="s">
-        <v>379</v>
+        <v>412</v>
       </c>
       <c r="C40" s="35" t="s">
-        <v>380</v>
+        <v>413</v>
       </c>
       <c r="D40" s="34" t="s">
         <v>129</v>
@@ -19240,10 +19465,10 @@
         <v>50050</v>
       </c>
       <c r="B41" s="178" t="s">
-        <v>381</v>
+        <v>414</v>
       </c>
       <c r="C41" s="178" t="s">
-        <v>382</v>
+        <v>415</v>
       </c>
       <c r="D41" s="158" t="s">
         <v>124</v>
@@ -19321,7 +19546,7 @@
         <v>40611</v>
       </c>
       <c r="B42" s="219" t="s">
-        <v>383</v>
+        <v>416</v>
       </c>
       <c r="C42" s="218" t="s">
         <v>56</v>
@@ -19479,10 +19704,10 @@
         <v>55165</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>384</v>
+        <v>417</v>
       </c>
       <c r="C44" s="35" t="s">
-        <v>385</v>
+        <v>418</v>
       </c>
       <c r="D44" s="34" t="s">
         <v>129</v>
@@ -19560,7 +19785,7 @@
         <v>40265</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>386</v>
+        <v>419</v>
       </c>
       <c r="C45" s="35" t="s">
         <v>27</v>
@@ -19639,7 +19864,7 @@
         <v>39543</v>
       </c>
       <c r="B46" s="219" t="s">
-        <v>387</v>
+        <v>420</v>
       </c>
       <c r="C46" s="218" t="s">
         <v>56</v>
@@ -19718,10 +19943,10 @@
         <v>39754</v>
       </c>
       <c r="B47" s="35" t="s">
-        <v>388</v>
+        <v>421</v>
       </c>
       <c r="C47" s="35" t="s">
-        <v>375</v>
+        <v>408</v>
       </c>
       <c r="D47" s="34" t="s">
         <v>124</v>
@@ -19955,7 +20180,7 @@
         <v>40582</v>
       </c>
       <c r="B50" s="35" t="s">
-        <v>389</v>
+        <v>422</v>
       </c>
       <c r="C50" s="35" t="s">
         <v>56</v>
@@ -20192,7 +20417,7 @@
         <v>41825</v>
       </c>
       <c r="B53" s="219" t="s">
-        <v>390</v>
+        <v>423</v>
       </c>
       <c r="C53" s="218" t="s">
         <v>27</v>
@@ -20350,10 +20575,10 @@
         <v>2015062906</v>
       </c>
       <c r="B55" s="75" t="s">
-        <v>391</v>
+        <v>424</v>
       </c>
       <c r="C55" s="81" t="s">
-        <v>392</v>
+        <v>425</v>
       </c>
       <c r="D55" s="85" t="s">
         <v>124</v>

</xml_diff>